<commit_message>
adjusted to account for biological replicates for the vesicle samples
</commit_message>
<xml_diff>
--- a/MetaDat/CellCount_fromLauraH.xlsx
+++ b/MetaDat/CellCount_fromLauraH.xlsx
@@ -1,16 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherineheal/Google_Drive/My Drive/4_OtherProjects/_Vesicles/DataProcessing_Vesicles/MetaDat/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EC1C84-4016-EA48-8C09-6ECEB05796E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1680" windowWidth="23920" windowHeight="15780" tabRatio="500"/>
+    <workbookView xWindow="1680" yWindow="1680" windowWidth="23920" windowHeight="15780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CellCount.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -153,7 +167,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -195,6 +209,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -519,22 +541,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16:W19"/>
+      <selection activeCell="V2" sqref="V2:V7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="33.1640625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="18" max="18" width="24.5" customWidth="1"/>
+    <col min="22" max="22" width="19.6640625" customWidth="1"/>
     <col min="25" max="25" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +643,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -710,7 +733,7 @@
         <v>1.7671458676442586</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -782,7 +805,7 @@
         <v>37123153.18991939</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -854,7 +877,7 @@
         <v>37175513.067479223</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -926,7 +949,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1006,7 +1029,7 @@
         <v>421.87499999999989</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>

</xml_diff>